<commit_message>
Actualizacion de datos 17/07/2025
</commit_message>
<xml_diff>
--- a/AnalisisCSV.xlsx
+++ b/AnalisisCSV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://telefonicacorp-my.sharepoint.com/personal/andres_palaciosgarcia_telefonica_com/Documents/ProyectosPython/CSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="8_{17429488-FBEC-48A3-BD93-E16729586F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4424FC29-155B-4677-A26F-E1EA3665DC75}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="8_{17429488-FBEC-48A3-BD93-E16729586F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6931BCD9-19C7-4415-A13E-B912DF9AFB3C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{52D8D840-2724-46EB-894B-880FF9A5A168}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{52D8D840-2724-46EB-894B-880FF9A5A168}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla dinamica" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="50">
   <si>
     <t>producto</t>
   </si>
@@ -197,10 +197,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -683,7 +689,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -881,7 +887,7 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:overlap val="100"/>
         <c:axId val="176244048"/>
         <c:axId val="493506368"/>
       </c:barChart>
@@ -1507,7 +1513,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1518,7 +1524,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>luz</c:v>
+                  <c:v>gas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1535,28 +1541,31 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Tabla dinamica'!$I$11:$I$18</c:f>
+              <c:f>'Tabla dinamica'!$I$11:$I$19</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2019</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2020</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2021</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2022</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2023</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2024</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2025</c:v>
                 </c:pt>
               </c:strCache>
@@ -1564,29 +1573,124 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tabla dinamica'!$J$11:$J$18</c:f>
+              <c:f>'Tabla dinamica'!$J$11:$J$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>5206</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15455</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15227</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16182</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13560</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7582.04</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12914.939999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4470</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B8C9-4F90-AB58-3720E7D67E66}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Tabla dinamica'!$K$9:$K$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>luz</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Tabla dinamica'!$I$11:$I$19</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2025</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Tabla dinamica'!$K$11:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="1">
                   <c:v>1465</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>2220</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2618</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1298</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1836</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3090</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>300.22000000000003</c:v>
                 </c:pt>
               </c:numCache>
@@ -1594,7 +1698,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B8C9-4F90-AB58-3720E7D67E66}"/>
+              <c16:uniqueId val="{00000000-3CA2-450A-99C0-F0CC007810F4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1607,7 +1711,7 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:overlap val="100"/>
         <c:axId val="67606992"/>
         <c:axId val="67607472"/>
       </c:barChart>
@@ -5779,7 +5883,318 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{450531B3-ECD3-4E63-976E-519BEC3A5BBC}" name="TablaDinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5102019C-0510-42C8-8FCB-227A3789E8A3}" name="TablaDinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="I9:L19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item h="1" x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0">
+      <items count="114">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="35"/>
+        <item x="34"/>
+        <item x="36"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="37"/>
+        <item x="41"/>
+        <item x="40"/>
+        <item x="43"/>
+        <item x="42"/>
+        <item x="44"/>
+        <item x="47"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="48"/>
+        <item x="51"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="52"/>
+        <item x="55"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="62"/>
+        <item x="61"/>
+        <item x="63"/>
+        <item x="65"/>
+        <item x="64"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="71"/>
+        <item x="69"/>
+        <item x="72"/>
+        <item x="70"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="76"/>
+        <item x="75"/>
+        <item x="81"/>
+        <item x="78"/>
+        <item x="77"/>
+        <item x="79"/>
+        <item x="82"/>
+        <item x="80"/>
+        <item x="85"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="86"/>
+        <item x="89"/>
+        <item x="88"/>
+        <item x="87"/>
+        <item x="91"/>
+        <item x="93"/>
+        <item x="90"/>
+        <item x="92"/>
+        <item x="94"/>
+        <item x="108"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="99"/>
+        <item x="104"/>
+        <item x="98"/>
+        <item x="100"/>
+        <item x="101"/>
+        <item x="102"/>
+        <item x="105"/>
+        <item x="103"/>
+        <item x="106"/>
+        <item x="107"/>
+        <item x="109"/>
+        <item x="110"/>
+        <item x="111"/>
+        <item x="112"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="14">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="10">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="13"/>
+    <field x="12"/>
+    <field x="11"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de kwh" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="6">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{450531B3-ECD3-4E63-976E-519BEC3A5BBC}" name="TablaDinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:D13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField axis="axisCol" showAll="0">
@@ -6089,311 +6504,6 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5102019C-0510-42C8-8FCB-227A3789E8A3}" name="TablaDinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="I9:K18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item h="1" x="2"/>
-        <item h="1" x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField axis="axisRow" numFmtId="14" showAll="0">
-      <items count="114">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="35"/>
-        <item x="34"/>
-        <item x="36"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="37"/>
-        <item x="41"/>
-        <item x="40"/>
-        <item x="43"/>
-        <item x="42"/>
-        <item x="44"/>
-        <item x="47"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="48"/>
-        <item x="51"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="52"/>
-        <item x="55"/>
-        <item x="53"/>
-        <item x="54"/>
-        <item x="56"/>
-        <item x="57"/>
-        <item x="58"/>
-        <item x="59"/>
-        <item x="60"/>
-        <item x="62"/>
-        <item x="61"/>
-        <item x="63"/>
-        <item x="65"/>
-        <item x="64"/>
-        <item x="66"/>
-        <item x="67"/>
-        <item x="68"/>
-        <item x="71"/>
-        <item x="69"/>
-        <item x="72"/>
-        <item x="70"/>
-        <item x="73"/>
-        <item x="74"/>
-        <item x="76"/>
-        <item x="75"/>
-        <item x="81"/>
-        <item x="78"/>
-        <item x="77"/>
-        <item x="79"/>
-        <item x="82"/>
-        <item x="80"/>
-        <item x="85"/>
-        <item x="83"/>
-        <item x="84"/>
-        <item x="86"/>
-        <item x="89"/>
-        <item x="88"/>
-        <item x="87"/>
-        <item x="91"/>
-        <item x="93"/>
-        <item x="90"/>
-        <item x="92"/>
-        <item x="94"/>
-        <item x="108"/>
-        <item x="95"/>
-        <item x="96"/>
-        <item x="97"/>
-        <item x="99"/>
-        <item x="104"/>
-        <item x="98"/>
-        <item x="100"/>
-        <item x="101"/>
-        <item x="102"/>
-        <item x="105"/>
-        <item x="103"/>
-        <item x="106"/>
-        <item x="107"/>
-        <item x="109"/>
-        <item x="110"/>
-        <item x="111"/>
-        <item x="112"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="14">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" x="10"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="13"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="10">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="4">
-    <field x="13"/>
-    <field x="12"/>
-    <field x="11"/>
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Suma de kwh" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="6">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A7D9493-C935-4C68-B498-259DC7F81BCF}" name="Tabla2" displayName="Tabla2" ref="A1:D7" totalsRowShown="0">
   <autoFilter ref="A1:D7" xr:uid="{2A7D9493-C935-4C68-B498-259DC7F81BCF}"/>
@@ -6410,8 +6520,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A31202E4-4761-4D69-822D-B4F7E3414C64}" name="Tabla1" displayName="Tabla1" ref="A1:K119" totalsRowShown="0">
-  <autoFilter ref="A1:K119" xr:uid="{A31202E4-4761-4D69-822D-B4F7E3414C64}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A31202E4-4761-4D69-822D-B4F7E3414C64}" name="Tabla1" displayName="Tabla1" ref="A1:K122" totalsRowShown="0">
+  <autoFilter ref="A1:K122" xr:uid="{A31202E4-4761-4D69-822D-B4F7E3414C64}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="agua"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{894F7388-A01F-4D74-96CB-2FF5F9052A60}" name="producto"/>
     <tableColumn id="2" xr3:uid="{CA29111B-EADA-408D-9B9D-7F5F070916B1}" name="Inicio" dataDxfId="1"/>
@@ -6728,10 +6844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7E7585-0700-498F-A9C0-C3F6621D9D2F}">
-  <dimension ref="A3:K18"/>
+  <dimension ref="A3:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6742,10 +6858,11 @@
     <col min="4" max="5" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
@@ -6753,7 +6870,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -6767,7 +6884,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>35</v>
       </c>
@@ -6779,7 +6896,7 @@
         <v>352.47</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -6800,7 +6917,7 @@
         <v>222.67999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
@@ -6814,7 +6931,7 @@
         <v>1773.0800000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -6828,7 +6945,7 @@
         <v>1859.81</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
@@ -6848,7 +6965,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -6865,13 +6982,16 @@
         <v>33</v>
       </c>
       <c r="J10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" t="s">
         <v>6</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
@@ -6885,16 +7005,17 @@
         <v>1533.1</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J11" s="4">
-        <v>1465</v>
-      </c>
-      <c r="K11" s="4">
-        <v>1465</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>5206</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4">
+        <v>5206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -6908,16 +7029,19 @@
         <v>369.05999999999995</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J12" s="4">
-        <v>2220</v>
+        <v>15455</v>
       </c>
       <c r="K12" s="4">
-        <v>2220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>1465</v>
+      </c>
+      <c r="L12" s="4">
+        <v>16920</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
@@ -6931,68 +7055,100 @@
         <v>9911</v>
       </c>
       <c r="I13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="4">
+        <v>15227</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2220</v>
+      </c>
+      <c r="L13" s="4">
+        <v>17447</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J14" s="4">
+        <v>16182</v>
+      </c>
+      <c r="K14" s="4">
         <v>2618</v>
       </c>
-      <c r="K13" s="4">
-        <v>2618</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I14" s="3" t="s">
+      <c r="L14" s="4">
+        <v>18800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J15" s="4">
+        <v>13560</v>
+      </c>
+      <c r="K15" s="4">
         <v>1298</v>
       </c>
-      <c r="K14" s="4">
-        <v>1298</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I15" s="3" t="s">
+      <c r="L15" s="4">
+        <v>14858</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J16" s="4">
+        <v>7582.04</v>
+      </c>
+      <c r="K16" s="4">
         <v>1836</v>
       </c>
-      <c r="K15" s="4">
-        <v>1836</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I16" s="3" t="s">
+      <c r="L16" s="4">
+        <v>9418.0400000000009</v>
+      </c>
+    </row>
+    <row r="17" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J17" s="4">
+        <v>12914.939999999999</v>
+      </c>
+      <c r="K17" s="4">
         <v>3090</v>
       </c>
-      <c r="K16" s="4">
-        <v>3090</v>
-      </c>
-    </row>
-    <row r="17" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I17" s="3" t="s">
+      <c r="L17" s="4">
+        <v>16004.939999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J18" s="4">
+        <v>4470</v>
+      </c>
+      <c r="K18" s="4">
         <v>300.22000000000003</v>
       </c>
-      <c r="K17" s="4">
-        <v>300.22000000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="I18" s="3" t="s">
+      <c r="L18" s="4">
+        <v>4770.22</v>
+      </c>
+    </row>
+    <row r="19" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I19" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J19" s="4">
+        <v>90596.98</v>
+      </c>
+      <c r="K19" s="4">
         <v>12827.22</v>
       </c>
-      <c r="K18" s="4">
-        <v>12827.22</v>
+      <c r="L19" s="4">
+        <v>103424.20000000001</v>
       </c>
     </row>
   </sheetData>
@@ -7126,10 +7282,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39AC097-4782-42D7-B6D7-CFEAC10EEA53}">
-  <dimension ref="A1:K119"/>
+  <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7173,7 +7329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7209,7 +7365,7 @@
         <v>2.1215942028985504</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -7245,7 +7401,7 @@
         <v>0.68096774193548382</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -7281,7 +7437,7 @@
         <v>0.72309090909090912</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -7317,7 +7473,7 @@
         <v>1.9696825396825397</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -7353,7 +7509,7 @@
         <v>4.8925000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -7389,7 +7545,7 @@
         <v>1.7631034482758621</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -7425,7 +7581,7 @@
         <v>5.6518965517241382</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -7461,7 +7617,7 @@
         <v>1.6037704918032787</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -7497,7 +7653,7 @@
         <v>2.988548387096774</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -7533,7 +7689,7 @@
         <v>1.6451666666666667</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -7569,7 +7725,7 @@
         <v>1.8883333333333334</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -7605,7 +7761,7 @@
         <v>1.5319047619047619</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -7641,7 +7797,7 @@
         <v>0.6204615384615384</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -7677,7 +7833,7 @@
         <v>1.6001666666666667</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -7713,7 +7869,7 @@
         <v>2.5046666666666666</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -7749,7 +7905,7 @@
         <v>1.6569354838709678</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -7785,7 +7941,7 @@
         <v>6.0203125000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -7821,7 +7977,7 @@
         <v>1.6778333333333333</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -7857,7 +8013,7 @@
         <v>5.3759322033898309</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -7893,7 +8049,7 @@
         <v>1.8488524590163935</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -7929,7 +8085,7 @@
         <v>3.0550819672131149</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -7965,7 +8121,7 @@
         <v>1.6570491803278689</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -8001,7 +8157,7 @@
         <v>0.85409836065573774</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -8037,7 +8193,7 @@
         <v>2.2214285714285711</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -8073,7 +8229,7 @@
         <v>0.77322033898305076</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -8109,7 +8265,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -8145,7 +8301,7 @@
         <v>2.1918333333333333</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -8181,7 +8337,7 @@
         <v>2.1477049180327867</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -8217,7 +8373,7 @@
         <v>7.2245454545454546</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -8253,7 +8409,7 @@
         <v>2.0824137931034481</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -8289,7 +8445,7 @@
         <v>5.3345901639344264</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -8325,7 +8481,7 @@
         <v>1.9596774193548387</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -8361,7 +8517,7 @@
         <v>3.1192307692307688</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -8397,7 +8553,7 @@
         <v>1.861578947368421</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -8433,7 +8589,7 @@
         <v>0.69016949152542373</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -8469,7 +8625,7 @@
         <v>1.4622857142857142</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -8505,7 +8661,7 @@
         <v>0.82777777777777783</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -8541,7 +8697,7 @@
         <v>0.64873239436619723</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -8577,7 +8733,7 @@
         <v>1.4392857142857143</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -8613,7 +8769,7 @@
         <v>2.0784375000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -8649,7 +8805,7 @@
         <v>1.1153333333333333</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -8685,7 +8841,7 @@
         <v>2.2333333333333334</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -8721,7 +8877,7 @@
         <v>2.3185714285714285</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -8757,7 +8913,7 @@
         <v>1.1340000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -8793,7 +8949,7 @@
         <v>1.2811538461538463</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -8859,7 +9015,7 @@
         <v>0.84499999999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -8895,7 +9051,7 @@
         <v>1.3788888888888888</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -8931,7 +9087,7 @@
         <v>1.556</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -8997,7 +9153,7 @@
         <v>0.74298245614035086</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -9033,7 +9189,7 @@
         <v>1.4643999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -9069,7 +9225,7 @@
         <v>1.3903333333333334</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -9135,7 +9291,7 @@
         <v>0.74220338983050849</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -9171,7 +9327,7 @@
         <v>1.264</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -9207,7 +9363,7 @@
         <v>1.1738709677419354</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -9273,7 +9429,7 @@
         <v>0.84539682539682537</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -9369,7 +9525,7 @@
         <v>0.87311475409836059</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -9405,7 +9561,7 @@
         <v>1.7872340425531914</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -9441,7 +9597,7 @@
         <v>4.5719047619047624</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -9477,7 +9633,7 @@
         <v>1.3233333333333335</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -9509,11 +9665,11 @@
         <v>5.5</v>
       </c>
       <c r="K67">
-        <f t="shared" ref="K67:K119" si="1">E67/D67</f>
+        <f t="shared" ref="K67:K122" si="1">E67/D67</f>
         <v>1.0709677419354839</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -9579,7 +9735,7 @@
         <v>0.74661290322580642</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -9615,7 +9771,7 @@
         <v>1.1810344827586208</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -9651,7 +9807,7 @@
         <v>1.1236363636363635</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -9687,7 +9843,7 @@
         <v>2.1085714285714285</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -9753,7 +9909,7 @@
         <v>1.5246666666666668</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -9789,7 +9945,7 @@
         <v>0.61333333333333329</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -9825,7 +9981,7 @@
         <v>1.9170967741935483</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -9921,7 +10077,7 @@
         <v>0.75032258064516133</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -9957,7 +10113,7 @@
         <v>1.3044827586206895</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -9993,7 +10149,7 @@
         <v>1.3009999999999999</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -10029,7 +10185,7 @@
         <v>1.453125</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -10065,7 +10221,7 @@
         <v>0.21237288135593219</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>5</v>
       </c>
@@ -10101,7 +10257,7 @@
         <v>2.8282258064516128</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -10137,7 +10293,7 @@
         <v>1.3440000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -10203,7 +10359,7 @@
         <v>0.59532258064516119</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -10239,7 +10395,7 @@
         <v>1.4216666666666666</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -10275,7 +10431,7 @@
         <v>1.7539285714285715</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -10371,7 +10527,7 @@
         <v>0.84333333333333338</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -10407,7 +10563,7 @@
         <v>1.4289999999999998</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>5</v>
       </c>
@@ -10443,7 +10599,7 @@
         <v>0.70627450980392159</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -10479,7 +10635,7 @@
         <v>1.3533333333333333</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -10515,7 +10671,7 @@
         <v>1.3444117647058824</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -10581,7 +10737,7 @@
         <v>2.9506451612903226</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -10647,7 +10803,7 @@
         <v>2.2650000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>5</v>
       </c>
@@ -10683,7 +10839,7 @@
         <v>0.42354838709677423</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -10719,7 +10875,7 @@
         <v>1.8712903225806452</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>5</v>
       </c>
@@ -10755,7 +10911,7 @@
         <v>0.30140350877192984</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -10791,7 +10947,7 @@
         <v>1.8712903225806452</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -10857,7 +11013,7 @@
         <v>0.62278688524590164</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -10893,7 +11049,7 @@
         <v>2.1533333333333333</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -10929,7 +11085,7 @@
         <v>1.8712903225806452</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -10965,7 +11121,7 @@
         <v>0.6164705882352941</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -11001,7 +11157,7 @@
         <v>0.70333333333333337</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>5</v>
       </c>
@@ -11037,7 +11193,7 @@
         <v>2.2216071428571427</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>5</v>
       </c>
@@ -11073,7 +11229,7 @@
         <v>1.552</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>5</v>
       </c>
@@ -11109,7 +11265,7 @@
         <v>2.2216071428571427</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -11171,11 +11327,11 @@
         <v>0.49692307692307602</v>
       </c>
       <c r="K115">
-        <f t="shared" si="1"/>
+        <f>E115/D115</f>
         <v>0.49692307692307686</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>5</v>
       </c>
@@ -11211,7 +11367,7 @@
         <v>5.0911290322580642</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -11247,7 +11403,7 @@
         <v>0.85312500000000002</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -11285,41 +11441,141 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B119" s="1">
-        <v>45430</v>
+        <v>45660</v>
       </c>
       <c r="C119" s="1">
-        <v>45450</v>
+        <v>45720</v>
       </c>
       <c r="D119">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E119">
-        <v>31.04</v>
+        <v>38.79</v>
       </c>
       <c r="F119">
-        <v>4.0870488322717599E-2</v>
+        <v>2.04157894736842</v>
       </c>
       <c r="G119">
-        <v>471</v>
-      </c>
-      <c r="H119">
-        <v>4.6688599999999996</v>
-      </c>
-      <c r="I119">
-        <v>0.23344300000000001</v>
-      </c>
-      <c r="J119">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="K119">
         <f t="shared" si="1"/>
-        <v>1.552</v>
+        <v>0.64649999999999996</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120" s="1">
+        <v>45687</v>
+      </c>
+      <c r="C120" s="1">
+        <v>45748</v>
+      </c>
+      <c r="D120">
+        <v>61</v>
+      </c>
+      <c r="E120">
+        <v>295.18</v>
+      </c>
+      <c r="F120">
+        <v>5.5527714502657498E-2</v>
+      </c>
+      <c r="G120">
+        <v>3951</v>
+      </c>
+      <c r="H120">
+        <v>11.351001999999999</v>
+      </c>
+      <c r="I120">
+        <v>0.186082</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120">
+        <f t="shared" si="1"/>
+        <v>4.8390163934426234</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>6</v>
+      </c>
+      <c r="B121" s="1">
+        <v>45715</v>
+      </c>
+      <c r="C121" s="1">
+        <v>45743</v>
+      </c>
+      <c r="D121">
+        <v>28</v>
+      </c>
+      <c r="E121">
+        <v>23.9</v>
+      </c>
+      <c r="F121">
+        <v>0.13520710059171501</v>
+      </c>
+      <c r="G121">
+        <v>169</v>
+      </c>
+      <c r="H121">
+        <v>1.6</v>
+      </c>
+      <c r="I121">
+        <v>1.0389610389610299E-2</v>
+      </c>
+      <c r="J121">
+        <v>5.5</v>
+      </c>
+      <c r="K121">
+        <f t="shared" si="1"/>
+        <v>0.85357142857142854</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>6</v>
+      </c>
+      <c r="B122" s="1">
+        <v>45743</v>
+      </c>
+      <c r="C122" s="1">
+        <v>45775</v>
+      </c>
+      <c r="D122">
+        <v>32</v>
+      </c>
+      <c r="E122">
+        <v>20.84</v>
+      </c>
+      <c r="F122">
+        <v>0.108231292517006</v>
+      </c>
+      <c r="G122">
+        <v>147</v>
+      </c>
+      <c r="H122">
+        <v>1.84</v>
+      </c>
+      <c r="I122">
+        <v>1.04545454545454E-2</v>
+      </c>
+      <c r="J122">
+        <v>5.5</v>
+      </c>
+      <c r="K122">
+        <f t="shared" si="1"/>
+        <v>0.65125</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>